<commit_message>
Actualización 2 de abril de 2024 - Lap HP
Se actualiza el repositorio con el material del curso.
</commit_message>
<xml_diff>
--- a/Bitacoras/NRC_124_Grupo_43/Parcial_03/Bitacora_Evaluacion_Continua_Parcial_03_NRC_124.xlsx
+++ b/Bitacoras/NRC_124_Grupo_43/Parcial_03/Bitacora_Evaluacion_Continua_Parcial_03_NRC_124.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\Bitacoras\NRC_124_Grupo_43\Parcial_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C406C7-D541-463F-BB2A-5E6C0BB4F079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC208924-D828-4E6E-A87E-A96CE03F2D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{290973E0-6FF6-4F81-956C-5BFE21AE5B1E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{290973E0-6FF6-4F81-956C-5BFE21AE5B1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Satélites" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="89">
   <si>
     <t>Matrícula</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>Faltas</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -353,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +375,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -386,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -410,6 +419,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -741,7 +753,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1204,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -1205,7 +1217,7 @@
       </c>
       <c r="G19" s="1">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2178,7 +2190,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection sqref="A1:A30"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3170,8 +3182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8727DB94-4916-409C-9144-CE8D39448BC0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3702,9 +3714,27 @@
       <c r="A20" t="s">
         <v>20</v>
       </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.5</v>
+      </c>
       <c r="H20" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3712,26 +3742,26 @@
         <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -3932,8 +3962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A28C3D7-B5CE-4D7C-9DB9-0E39AEB35559}">
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4227,32 +4257,35 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
@@ -4261,16 +4294,16 @@
         <v>0</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4" s="1">
         <v>0</v>
@@ -4279,7 +4312,7 @@
         <v>0</v>
       </c>
       <c r="V4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="1">
         <v>0</v>
@@ -4289,14 +4322,15 @@
       </c>
       <c r="Y4" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="Z4" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA4" s="9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6.5</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -4389,11 +4423,11 @@
       </c>
       <c r="AD5" s="1">
         <f>COUNTIF(AA2:AA28,"&gt;=6")</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AE5" s="8">
         <f>AD5/25</f>
-        <v>0.68</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -4486,11 +4520,11 @@
       </c>
       <c r="AD6" s="9">
         <f>COUNTIF(AA2:AA28,"&lt;6")-2</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AE6" s="8">
         <f>AD6/25</f>
-        <v>0.32</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -6035,7 +6069,7 @@
         <v>9</v>
       </c>
       <c r="AA24" s="9">
-        <f t="shared" ref="AA24:AA27" si="3">IF(Z24=10,Z24,Z24+0.5)</f>
+        <f t="shared" ref="AA24:AA28" si="3">IF(Z24=10,Z24,Z24+0.5)</f>
         <v>9.5</v>
       </c>
     </row>
@@ -6307,35 +6341,38 @@
       <c r="C28" t="s">
         <v>30</v>
       </c>
+      <c r="D28" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="E28" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="1">
         <v>0</v>
       </c>
       <c r="L28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" s="1">
         <v>0</v>
       </c>
       <c r="N28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" s="1">
         <v>0</v>
@@ -6344,16 +6381,16 @@
         <v>0</v>
       </c>
       <c r="Q28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S28" s="1">
         <v>0</v>
       </c>
       <c r="T28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28" s="1">
         <v>0</v>
@@ -6362,21 +6399,22 @@
         <v>0</v>
       </c>
       <c r="W28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y28" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="Z28" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA28" s="9">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>
@@ -6387,13 +6425,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFEB7F98-1FFF-4EFC-8C0D-71BF12C18CD5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="7815" ySplit="1155" topLeftCell="I1" activePane="bottomRight"/>
+      <pane xSplit="7815" ySplit="1155" topLeftCell="H20" activePane="bottomLeft"/>
       <selection pane="topRight" activeCell="L2" sqref="L1:L1048576"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
-      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6478,7 +6517,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20263998</v>
       </c>
@@ -6491,35 +6530,35 @@
       <c r="D3" s="1">
         <v>4</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
+      <c r="E3" s="11">
+        <v>8</v>
+      </c>
+      <c r="F3" s="11">
+        <v>2</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
       <c r="H3" s="1">
         <f>SUM(C3:G3)</f>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="I3" s="9">
         <f>(H3/$H$1)*10</f>
-        <v>3.4615384615384617</v>
+        <v>7.3076923076923075</v>
       </c>
       <c r="J3" s="9">
         <v>5.5</v>
       </c>
       <c r="K3" s="9">
         <f>I3*0.4+J3*0.6</f>
-        <v>4.6846153846153848</v>
+        <v>6.2230769230769232</v>
       </c>
       <c r="L3" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20244739</v>
       </c>
@@ -6560,7 +6599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10186663</v>
       </c>
@@ -6591,17 +6630,17 @@
         <v>0</v>
       </c>
       <c r="J5" s="9">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="K5" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="L5" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10187045</v>
       </c>
@@ -6642,7 +6681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10186376</v>
       </c>
@@ -6683,7 +6722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20238395</v>
       </c>
@@ -6724,7 +6763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10185692</v>
       </c>
@@ -6765,7 +6804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20266322</v>
       </c>
@@ -6806,7 +6845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20245456</v>
       </c>
@@ -6846,7 +6885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10186574</v>
       </c>
@@ -6887,7 +6926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20249032</v>
       </c>
@@ -6928,7 +6967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20266998</v>
       </c>
@@ -6969,7 +7008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20264862</v>
       </c>
@@ -7010,7 +7049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20268353</v>
       </c>
@@ -7051,7 +7090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20264649</v>
       </c>
@@ -7092,7 +7131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10187502</v>
       </c>
@@ -7133,7 +7172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20235464</v>
       </c>
@@ -7182,7 +7221,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="1">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
         <v>4</v>
@@ -7198,24 +7237,23 @@
       </c>
       <c r="H20" s="1">
         <f t="shared" si="0"/>
-        <v>13.9</v>
+        <v>14.4</v>
       </c>
       <c r="I20" s="9">
-        <f t="shared" si="1"/>
-        <v>5.3461538461538458</v>
+        <v>6.12</v>
       </c>
       <c r="J20" s="9">
         <v>5</v>
       </c>
       <c r="K20" s="9">
         <f t="shared" si="2"/>
-        <v>5.138461538461538</v>
+        <v>5.4480000000000004</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20244756</v>
       </c>
@@ -7235,28 +7273,28 @@
         <v>2</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="0"/>
-        <v>17.399999999999999</v>
+        <v>22.4</v>
       </c>
       <c r="I21" s="9">
         <f t="shared" si="1"/>
-        <v>6.6923076923076916</v>
+        <v>8.615384615384615</v>
       </c>
       <c r="J21" s="9">
         <v>6</v>
       </c>
       <c r="K21" s="9">
         <f t="shared" si="2"/>
-        <v>6.2769230769230759</v>
+        <v>7.046153846153846</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20266315</v>
       </c>
@@ -7276,28 +7314,28 @@
         <v>2</v>
       </c>
       <c r="G22" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="0"/>
-        <v>17.3</v>
+        <v>22.3</v>
       </c>
       <c r="I22" s="9">
         <f t="shared" si="1"/>
-        <v>6.6538461538461551</v>
+        <v>8.5769230769230766</v>
       </c>
       <c r="J22" s="9">
         <v>0</v>
       </c>
       <c r="K22" s="9">
         <f t="shared" si="2"/>
-        <v>2.6615384615384623</v>
+        <v>3.430769230769231</v>
       </c>
       <c r="L22" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20271313</v>
       </c>
@@ -7338,7 +7376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20251515</v>
       </c>
@@ -7379,7 +7417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20250030</v>
       </c>
@@ -7396,31 +7434,31 @@
         <v>7.9</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G25" s="1">
         <v>7</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="0"/>
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="I25" s="9">
         <f t="shared" si="1"/>
-        <v>9.1923076923076916</v>
+        <v>9.9615384615384599</v>
       </c>
       <c r="J25" s="9">
         <v>9.5</v>
       </c>
       <c r="K25" s="9">
         <f t="shared" si="2"/>
-        <v>9.3769230769230774</v>
+        <v>9.684615384615384</v>
       </c>
       <c r="L25" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20266265</v>
       </c>
@@ -7461,7 +7499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20251561</v>
       </c>
@@ -7502,7 +7540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20270002</v>
       </c>
@@ -7543,7 +7581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10186676</v>
       </c>
@@ -7574,18 +7612,24 @@
         <v>9.615384615384615</v>
       </c>
       <c r="J29" s="9">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="K29" s="9">
         <f t="shared" si="2"/>
-        <v>3.8461538461538463</v>
+        <v>7.7461538461538462</v>
       </c>
       <c r="L29" s="1">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:L29" xr:uid="{FFEB7F98-1FFF-4EFC-8C0D-71BF12C18CD5}"/>
+  <autoFilter ref="A2:L29" xr:uid="{FFEB7F98-1FFF-4EFC-8C0D-71BF12C18CD5}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="GONZALEZ TALAVERA AXEL IZACHARD"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="C3:G29">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
@@ -7600,7 +7644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7871D383-96EF-40B0-BCA7-1BED6CDE7089}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualización 14 de abril 2024 - Lap HP
Se actualiza con material del curso y con los exámenes ordinarios, tabla de especificaciones, hoja de solución y guía de estudio.
</commit_message>
<xml_diff>
--- a/Bitacoras/NRC_124_Grupo_43/Parcial_03/Bitacora_Evaluacion_Continua_Parcial_03_NRC_124.xlsx
+++ b/Bitacoras/NRC_124_Grupo_43/Parcial_03/Bitacora_Evaluacion_Continua_Parcial_03_NRC_124.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\Bitacoras\NRC_124_Grupo_43\Parcial_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC208924-D828-4E6E-A87E-A96CE03F2D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857043D8-D825-475D-BFE0-B1353A283DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{290973E0-6FF6-4F81-956C-5BFE21AE5B1E}"/>
   </bookViews>
@@ -6425,13 +6425,12 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFEB7F98-1FFF-4EFC-8C0D-71BF12C18CD5}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="7815" ySplit="1155" topLeftCell="H20" activePane="bottomLeft"/>
+      <pane xSplit="7815" ySplit="1155" topLeftCell="H16" activePane="bottomLeft"/>
       <selection pane="topRight" activeCell="L2" sqref="L1:L1048576"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B29"/>
       <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -6517,7 +6516,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20263998</v>
       </c>
@@ -6558,7 +6557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20244739</v>
       </c>
@@ -6599,7 +6598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10186663</v>
       </c>
@@ -6640,7 +6639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10187045</v>
       </c>
@@ -6681,7 +6680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10186376</v>
       </c>
@@ -6722,7 +6721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20238395</v>
       </c>
@@ -6763,7 +6762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10185692</v>
       </c>
@@ -6804,7 +6803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20266322</v>
       </c>
@@ -6845,7 +6844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20245456</v>
       </c>
@@ -6885,7 +6884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10186574</v>
       </c>
@@ -6926,7 +6925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20249032</v>
       </c>
@@ -6967,7 +6966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20266998</v>
       </c>
@@ -7008,7 +7007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20264862</v>
       </c>
@@ -7049,7 +7048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20268353</v>
       </c>
@@ -7090,7 +7089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20264649</v>
       </c>
@@ -7131,7 +7130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10187502</v>
       </c>
@@ -7172,7 +7171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20235464</v>
       </c>
@@ -7253,7 +7252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20244756</v>
       </c>
@@ -7294,7 +7293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20266315</v>
       </c>
@@ -7335,7 +7334,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20271313</v>
       </c>
@@ -7376,7 +7375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20251515</v>
       </c>
@@ -7417,7 +7416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20250030</v>
       </c>
@@ -7458,7 +7457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20266265</v>
       </c>
@@ -7499,7 +7498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20251561</v>
       </c>
@@ -7540,7 +7539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20270002</v>
       </c>
@@ -7581,7 +7580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10186676</v>
       </c>
@@ -7623,13 +7622,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:L29" xr:uid="{FFEB7F98-1FFF-4EFC-8C0D-71BF12C18CD5}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="GONZALEZ TALAVERA AXEL IZACHARD"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:L29" xr:uid="{FFEB7F98-1FFF-4EFC-8C0D-71BF12C18CD5}"/>
   <conditionalFormatting sqref="C3:G29">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>

</xml_diff>